<commit_message>
better idea if in progress
</commit_message>
<xml_diff>
--- a/Regular QA/test_urls.xlsx
+++ b/Regular QA/test_urls.xlsx
@@ -462,7 +462,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +503,15 @@
       <c r="C2">
         <v>508</v>
       </c>
+      <c r="D2">
+        <v>570</v>
+      </c>
+      <c r="F2">
+        <v>368</v>
+      </c>
+      <c r="G2">
+        <v>369</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -514,6 +523,15 @@
       <c r="C3">
         <v>507</v>
       </c>
+      <c r="D3">
+        <v>585</v>
+      </c>
+      <c r="F3">
+        <v>370</v>
+      </c>
+      <c r="G3">
+        <v>371</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -525,6 +543,15 @@
       <c r="C4">
         <v>528</v>
       </c>
+      <c r="D4">
+        <v>586</v>
+      </c>
+      <c r="F4">
+        <v>235</v>
+      </c>
+      <c r="G4">
+        <v>236</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -536,6 +563,15 @@
       <c r="C5">
         <v>525</v>
       </c>
+      <c r="D5">
+        <v>588</v>
+      </c>
+      <c r="F5">
+        <v>281</v>
+      </c>
+      <c r="G5">
+        <v>284</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -547,6 +583,15 @@
       <c r="C6">
         <v>495</v>
       </c>
+      <c r="D6">
+        <v>587</v>
+      </c>
+      <c r="F6">
+        <v>490</v>
+      </c>
+      <c r="G6">
+        <v>489</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -558,6 +603,15 @@
       <c r="C7">
         <v>524</v>
       </c>
+      <c r="D7">
+        <v>589</v>
+      </c>
+      <c r="F7">
+        <v>283</v>
+      </c>
+      <c r="G7">
+        <v>286</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -569,6 +623,15 @@
       <c r="C8">
         <v>529</v>
       </c>
+      <c r="D8">
+        <v>590</v>
+      </c>
+      <c r="F8">
+        <v>233</v>
+      </c>
+      <c r="G8">
+        <v>234</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -580,6 +643,15 @@
       <c r="C9">
         <v>506</v>
       </c>
+      <c r="D9">
+        <v>591</v>
+      </c>
+      <c r="F9">
+        <v>372</v>
+      </c>
+      <c r="G9">
+        <v>373</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -591,6 +663,15 @@
       <c r="C10">
         <v>530</v>
       </c>
+      <c r="D10">
+        <v>592</v>
+      </c>
+      <c r="F10">
+        <v>231</v>
+      </c>
+      <c r="G10">
+        <v>232</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -602,6 +683,15 @@
       <c r="C11">
         <v>504</v>
       </c>
+      <c r="D11">
+        <v>593</v>
+      </c>
+      <c r="F11">
+        <v>383</v>
+      </c>
+      <c r="G11">
+        <v>384</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -613,6 +703,15 @@
       <c r="C12">
         <v>503</v>
       </c>
+      <c r="D12">
+        <v>594</v>
+      </c>
+      <c r="F12">
+        <v>391</v>
+      </c>
+      <c r="G12">
+        <v>392</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -624,6 +723,15 @@
       <c r="C13">
         <v>497</v>
       </c>
+      <c r="D13">
+        <v>596</v>
+      </c>
+      <c r="F13">
+        <v>433</v>
+      </c>
+      <c r="G13">
+        <v>436</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -635,6 +743,15 @@
       <c r="C14">
         <v>496</v>
       </c>
+      <c r="D14">
+        <v>595</v>
+      </c>
+      <c r="F14">
+        <v>434</v>
+      </c>
+      <c r="G14">
+        <v>435</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -646,6 +763,15 @@
       <c r="C15">
         <v>500</v>
       </c>
+      <c r="D15">
+        <v>597</v>
+      </c>
+      <c r="F15">
+        <v>410</v>
+      </c>
+      <c r="G15">
+        <v>408</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -657,8 +783,17 @@
       <c r="C16">
         <v>499</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>598</v>
+      </c>
+      <c r="F16">
+        <v>411</v>
+      </c>
+      <c r="G16">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -668,64 +803,157 @@
       <c r="C17">
         <v>509</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>599</v>
+      </c>
+      <c r="F17">
+        <v>348</v>
+      </c>
+      <c r="G17">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B18">
         <v>619</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>620</v>
+      </c>
+      <c r="D18">
+        <v>621</v>
+      </c>
+      <c r="F18">
+        <v>622</v>
+      </c>
+      <c r="G18">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B19">
         <v>545</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>552</v>
+      </c>
+      <c r="D19">
+        <v>601</v>
+      </c>
+      <c r="F19">
+        <v>559</v>
+      </c>
+      <c r="G19">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B20">
         <v>544</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>551</v>
+      </c>
+      <c r="D20">
+        <v>602</v>
+      </c>
+      <c r="F20">
+        <v>558</v>
+      </c>
+      <c r="G20">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B21">
         <v>624</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>631</v>
+      </c>
+      <c r="D21">
+        <v>632</v>
+      </c>
+      <c r="F21">
+        <v>639</v>
+      </c>
+      <c r="G21">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B22">
         <v>543</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>550</v>
+      </c>
+      <c r="D22">
+        <v>603</v>
+      </c>
+      <c r="F22">
+        <v>557</v>
+      </c>
+      <c r="G22">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B23">
         <v>625</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>630</v>
+      </c>
+      <c r="D23">
+        <v>633</v>
+      </c>
+      <c r="F23">
+        <v>638</v>
+      </c>
+      <c r="G23">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B24">
         <v>542</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>549</v>
+      </c>
+      <c r="D24">
+        <v>604</v>
+      </c>
+      <c r="F24">
+        <v>556</v>
+      </c>
+      <c r="G24">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -735,8 +963,17 @@
       <c r="C25">
         <v>527</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>613</v>
+      </c>
+      <c r="F25">
+        <v>277</v>
+      </c>
+      <c r="G25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -745,6 +982,15 @@
       </c>
       <c r="C26">
         <v>526</v>
+      </c>
+      <c r="D26">
+        <v>612</v>
+      </c>
+      <c r="F26">
+        <v>279</v>
+      </c>
+      <c r="G26">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added BSIV and MSV
</commit_message>
<xml_diff>
--- a/Regular QA/test_urls.xlsx
+++ b/Regular QA/test_urls.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>RT1</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>ML11_p</t>
+  </si>
+  <si>
+    <t>MSV</t>
+  </si>
+  <si>
+    <t>BSIV</t>
   </si>
 </sst>
 </file>
@@ -459,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,6 +997,46 @@
       </c>
       <c r="G26">
         <v>280</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>448</v>
+      </c>
+      <c r="C27">
+        <v>502</v>
+      </c>
+      <c r="D27">
+        <v>609</v>
+      </c>
+      <c r="F27">
+        <v>397</v>
+      </c>
+      <c r="G27">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>449</v>
+      </c>
+      <c r="C28">
+        <v>501</v>
+      </c>
+      <c r="D28">
+        <v>608</v>
+      </c>
+      <c r="F28">
+        <v>401</v>
+      </c>
+      <c r="G28">
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>